<commit_message>
added next slot column to scrape_bracket
</commit_message>
<xml_diff>
--- a/predict.xlsx
+++ b/predict.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="682" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="682" uniqueCount="173">
   <si>
     <t>Index</t>
   </si>
@@ -52,6 +52,12 @@
     <t>Pick</t>
   </si>
   <si>
+    <t>16</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
     <t>01</t>
   </si>
   <si>
@@ -79,10 +85,16 @@
     <t>?</t>
   </si>
   <si>
-    <t>16</t>
-  </si>
-  <si>
-    <t>10</t>
+    <t>Howard</t>
+  </si>
+  <si>
+    <t>Colorado St.</t>
+  </si>
+  <si>
+    <t>Grambling St.</t>
+  </si>
+  <si>
+    <t>Colorado</t>
   </si>
   <si>
     <t>Connecticut</t>
@@ -157,7 +169,7 @@
     <t>Arizona</t>
   </si>
   <si>
-    <t>Purdue</t>
+    <t>56%</t>
   </si>
   <si>
     <t>Utah St.</t>
@@ -181,16 +193,16 @@
     <t>Tennessee</t>
   </si>
   <si>
-    <t>Howard</t>
-  </si>
-  <si>
-    <t>Colorado St.</t>
-  </si>
-  <si>
-    <t>Grambling St.</t>
-  </si>
-  <si>
-    <t>Colorado</t>
+    <t>54%</t>
+  </si>
+  <si>
+    <t>62%</t>
+  </si>
+  <si>
+    <t>44%</t>
+  </si>
+  <si>
+    <t>57%</t>
   </si>
   <si>
     <t>99%</t>
@@ -208,48 +220,45 @@
     <t>75%</t>
   </si>
   <si>
-    <t>54%</t>
-  </si>
-  <si>
     <t>93%</t>
   </si>
   <si>
+    <t>97%</t>
+  </si>
+  <si>
+    <t>51%</t>
+  </si>
+  <si>
+    <t>68%</t>
+  </si>
+  <si>
+    <t>53%</t>
+  </si>
+  <si>
+    <t>84%</t>
+  </si>
+  <si>
+    <t>91%</t>
+  </si>
+  <si>
+    <t>42%</t>
+  </si>
+  <si>
+    <t>61%</t>
+  </si>
+  <si>
+    <t>89%</t>
+  </si>
+  <si>
+    <t>52%</t>
+  </si>
+  <si>
+    <t>96%</t>
+  </si>
+  <si>
     <t>?%</t>
   </si>
   <si>
-    <t>97%</t>
-  </si>
-  <si>
-    <t>51%</t>
-  </si>
-  <si>
-    <t>68%</t>
-  </si>
-  <si>
-    <t>53%</t>
-  </si>
-  <si>
-    <t>84%</t>
-  </si>
-  <si>
-    <t>91%</t>
-  </si>
-  <si>
-    <t>42%</t>
-  </si>
-  <si>
-    <t>61%</t>
-  </si>
-  <si>
-    <t>89%</t>
-  </si>
-  <si>
-    <t>52%</t>
-  </si>
-  <si>
-    <t>96%</t>
-  </si>
-  <si>
     <t>47%</t>
   </si>
   <si>
@@ -262,21 +271,18 @@
     <t>50%</t>
   </si>
   <si>
-    <t>62%</t>
-  </si>
-  <si>
-    <t>44%</t>
-  </si>
-  <si>
-    <t>57%</t>
+    <t>65</t>
+  </si>
+  <si>
+    <t>66</t>
+  </si>
+  <si>
+    <t>68</t>
   </si>
   <si>
     <t>79</t>
   </si>
   <si>
-    <t>66</t>
-  </si>
-  <si>
     <t>71</t>
   </si>
   <si>
@@ -292,16 +298,10 @@
     <t>75</t>
   </si>
   <si>
-    <t>68</t>
-  </si>
-  <si>
     <t>70</t>
   </si>
   <si>
-    <t>78</t>
-  </si>
-  <si>
-    <t>65</t>
+    <t>81</t>
   </si>
   <si>
     <t>77</t>
@@ -310,9 +310,6 @@
     <t>73</t>
   </si>
   <si>
-    <t>81</t>
-  </si>
-  <si>
     <t>69</t>
   </si>
   <si>
@@ -334,6 +331,18 @@
     <t>15</t>
   </si>
   <si>
+    <t>Wagner</t>
+  </si>
+  <si>
+    <t>Virginia</t>
+  </si>
+  <si>
+    <t>Montana St.</t>
+  </si>
+  <si>
+    <t>Boise St.</t>
+  </si>
+  <si>
     <t>Stetson</t>
   </si>
   <si>
@@ -379,9 +388,6 @@
     <t>Western Kentucky</t>
   </si>
   <si>
-    <t>Wagner</t>
-  </si>
-  <si>
     <t>Michigan St.</t>
   </si>
   <si>
@@ -421,13 +427,13 @@
     <t>Saint Peter's</t>
   </si>
   <si>
-    <t>Virginia</t>
-  </si>
-  <si>
-    <t>Montana St.</t>
-  </si>
-  <si>
-    <t>Boise St.</t>
+    <t>46%</t>
+  </si>
+  <si>
+    <t>38%</t>
+  </si>
+  <si>
+    <t>43%</t>
   </si>
   <si>
     <t>1%</t>
@@ -442,9 +448,6 @@
     <t>25%</t>
   </si>
   <si>
-    <t>46%</t>
-  </si>
-  <si>
     <t>7%</t>
   </si>
   <si>
@@ -481,13 +484,10 @@
     <t>30%</t>
   </si>
   <si>
-    <t>38%</t>
-  </si>
-  <si>
-    <t>56%</t>
-  </si>
-  <si>
-    <t>43%</t>
+    <t>64</t>
+  </si>
+  <si>
+    <t>61</t>
   </si>
   <si>
     <t>52</t>
@@ -496,12 +496,6 @@
     <t>63</t>
   </si>
   <si>
-    <t>61</t>
-  </si>
-  <si>
-    <t>64</t>
-  </si>
-  <si>
     <t>60</t>
   </si>
   <si>
@@ -511,7 +505,7 @@
     <t>58</t>
   </si>
   <si>
-    <t>54</t>
+    <t>57</t>
   </si>
   <si>
     <t>59</t>
@@ -520,10 +514,7 @@
     <t>62</t>
   </si>
   <si>
-    <t>53</t>
-  </si>
-  <si>
-    <t>57</t>
+    <t>First Four</t>
   </si>
   <si>
     <t>EAST</t>
@@ -532,19 +523,16 @@
     <t>SOUTH</t>
   </si>
   <si>
+    <t>WEST</t>
+  </si>
+  <si>
+    <t>MIDWEST</t>
+  </si>
+  <si>
     <t>Final Four</t>
   </si>
   <si>
     <t>Championship</t>
-  </si>
-  <si>
-    <t>WEST</t>
-  </si>
-  <si>
-    <t>MIDWEST</t>
-  </si>
-  <si>
-    <t>First Four</t>
   </si>
 </sst>
 </file>
@@ -948,7 +936,7 @@
     </row>
     <row r="2" spans="1:12">
       <c r="A2">
-        <v>1</v>
+        <v>64</v>
       </c>
       <c r="B2" t="s">
         <v>12</v>
@@ -963,22 +951,22 @@
         <v>85</v>
       </c>
       <c r="F2" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="G2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="I2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="J2" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="K2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L2" t="s">
         <v>2</v>
@@ -986,7 +974,7 @@
     </row>
     <row r="3" spans="1:12">
       <c r="A3">
-        <v>2</v>
+        <v>65</v>
       </c>
       <c r="B3" t="s">
         <v>13</v>
@@ -998,36 +986,36 @@
         <v>60</v>
       </c>
       <c r="E3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F3" t="s">
-        <v>100</v>
+        <v>13</v>
       </c>
       <c r="G3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H3" t="s">
-        <v>76</v>
+        <v>138</v>
       </c>
       <c r="I3" t="s">
-        <v>86</v>
+        <v>157</v>
       </c>
       <c r="J3" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="K3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L3" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:12">
       <c r="A4">
-        <v>3</v>
+        <v>66</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C4" t="s">
         <v>25</v>
@@ -1036,36 +1024,36 @@
         <v>61</v>
       </c>
       <c r="E4" t="s">
+        <v>86</v>
+      </c>
+      <c r="F4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" t="s">
+        <v>107</v>
+      </c>
+      <c r="H4" t="s">
+        <v>51</v>
+      </c>
+      <c r="I4" t="s">
         <v>87</v>
       </c>
-      <c r="F4" t="s">
-        <v>101</v>
-      </c>
-      <c r="G4" t="s">
-        <v>108</v>
-      </c>
-      <c r="H4" t="s">
-        <v>139</v>
-      </c>
-      <c r="I4" t="s">
-        <v>159</v>
-      </c>
       <c r="J4" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="K4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L4" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:12">
       <c r="A5">
-        <v>4</v>
+        <v>67</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C5" t="s">
         <v>26</v>
@@ -1074,25 +1062,25 @@
         <v>62</v>
       </c>
       <c r="E5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F5" t="s">
-        <v>102</v>
+        <v>13</v>
       </c>
       <c r="G5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="H5" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="I5" t="s">
-        <v>160</v>
+        <v>86</v>
       </c>
       <c r="J5" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="K5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L5" t="s">
         <v>2</v>
@@ -1100,10 +1088,10 @@
     </row>
     <row r="6" spans="1:12">
       <c r="A6">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B6" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C6" t="s">
         <v>27</v>
@@ -1112,22 +1100,22 @@
         <v>63</v>
       </c>
       <c r="E6" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="F6" t="s">
-        <v>103</v>
+        <v>12</v>
       </c>
       <c r="G6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="H6" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="I6" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="J6" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="K6">
         <v>1</v>
@@ -1138,34 +1126,34 @@
     </row>
     <row r="7" spans="1:12">
       <c r="A7">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B7" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C7" t="s">
         <v>28</v>
       </c>
       <c r="D7" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="E7" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="F7" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="G7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="H7" t="s">
-        <v>140</v>
+        <v>78</v>
       </c>
       <c r="I7" t="s">
-        <v>160</v>
+        <v>86</v>
       </c>
       <c r="J7" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="K7">
         <v>1</v>
@@ -1176,34 +1164,34 @@
     </row>
     <row r="8" spans="1:12">
       <c r="A8">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B8" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C8" t="s">
         <v>29</v>
       </c>
       <c r="D8" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E8" t="s">
         <v>89</v>
       </c>
       <c r="F8" t="s">
-        <v>22</v>
+        <v>100</v>
       </c>
       <c r="G8" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H8" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="I8" t="s">
-        <v>86</v>
+        <v>159</v>
       </c>
       <c r="J8" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="K8">
         <v>1</v>
@@ -1214,34 +1202,34 @@
     </row>
     <row r="9" spans="1:12">
       <c r="A9">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B9" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C9" t="s">
         <v>30</v>
       </c>
       <c r="D9" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E9" t="s">
         <v>90</v>
       </c>
       <c r="F9" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="G9" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="H9" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="I9" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="J9" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="K9">
         <v>1</v>
@@ -1252,300 +1240,300 @@
     </row>
     <row r="10" spans="1:12">
       <c r="A10">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B10" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C10" t="s">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="D10" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E10" t="s">
-        <v>20</v>
+        <v>89</v>
       </c>
       <c r="F10" t="s">
-        <v>20</v>
+        <v>102</v>
       </c>
       <c r="G10" t="s">
-        <v>20</v>
+        <v>113</v>
       </c>
       <c r="H10" t="s">
-        <v>66</v>
+        <v>143</v>
       </c>
       <c r="I10" t="s">
-        <v>20</v>
+        <v>156</v>
       </c>
       <c r="J10" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="K10">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L10" t="s">
-        <v>20</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:12">
       <c r="A11">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C11" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="D11" t="s">
         <v>66</v>
       </c>
       <c r="E11" t="s">
-        <v>20</v>
+        <v>90</v>
       </c>
       <c r="F11" t="s">
-        <v>20</v>
+        <v>103</v>
       </c>
       <c r="G11" t="s">
-        <v>20</v>
+        <v>114</v>
       </c>
       <c r="H11" t="s">
-        <v>66</v>
+        <v>142</v>
       </c>
       <c r="I11" t="s">
-        <v>20</v>
+        <v>157</v>
       </c>
       <c r="J11" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="K11">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L11" t="s">
-        <v>20</v>
+        <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:12">
       <c r="A12">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B12" t="s">
         <v>20</v>
       </c>
       <c r="C12" t="s">
-        <v>20</v>
+        <v>33</v>
       </c>
       <c r="D12" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="E12" t="s">
-        <v>20</v>
+        <v>91</v>
       </c>
       <c r="F12" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="G12" t="s">
-        <v>20</v>
+        <v>115</v>
       </c>
       <c r="H12" t="s">
-        <v>66</v>
+        <v>137</v>
       </c>
       <c r="I12" t="s">
-        <v>20</v>
+        <v>86</v>
       </c>
       <c r="J12" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="K12">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L12" t="s">
-        <v>20</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:12">
       <c r="A13">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B13" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C13" t="s">
-        <v>20</v>
+        <v>34</v>
       </c>
       <c r="D13" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="E13" t="s">
-        <v>20</v>
+        <v>92</v>
       </c>
       <c r="F13" t="s">
-        <v>20</v>
+        <v>104</v>
       </c>
       <c r="G13" t="s">
-        <v>20</v>
+        <v>116</v>
       </c>
       <c r="H13" t="s">
-        <v>66</v>
+        <v>144</v>
       </c>
       <c r="I13" t="s">
-        <v>20</v>
+        <v>160</v>
       </c>
       <c r="J13" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="K13">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L13" t="s">
-        <v>20</v>
+        <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:12">
       <c r="A14">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B14" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="C14" t="s">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="D14" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="E14" t="s">
-        <v>20</v>
+        <v>93</v>
       </c>
       <c r="F14" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="G14" t="s">
-        <v>20</v>
+        <v>117</v>
       </c>
       <c r="H14" t="s">
-        <v>66</v>
+        <v>145</v>
       </c>
       <c r="I14" t="s">
-        <v>20</v>
+        <v>161</v>
       </c>
       <c r="J14" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="K14">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="L14" t="s">
-        <v>20</v>
+        <v>2</v>
       </c>
     </row>
     <row r="15" spans="1:12">
       <c r="A15">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B15" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="C15" t="s">
-        <v>20</v>
+        <v>36</v>
       </c>
       <c r="D15" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="E15" t="s">
-        <v>20</v>
+        <v>87</v>
       </c>
       <c r="F15" t="s">
-        <v>20</v>
+        <v>99</v>
       </c>
       <c r="G15" t="s">
-        <v>20</v>
+        <v>118</v>
       </c>
       <c r="H15" t="s">
-        <v>66</v>
+        <v>146</v>
       </c>
       <c r="I15" t="s">
-        <v>20</v>
+        <v>87</v>
       </c>
       <c r="J15" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="K15">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="L15" t="s">
-        <v>20</v>
+        <v>2</v>
       </c>
     </row>
     <row r="16" spans="1:12">
       <c r="A16">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B16" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C16" t="s">
-        <v>20</v>
+        <v>37</v>
       </c>
       <c r="D16" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="E16" t="s">
-        <v>20</v>
+        <v>94</v>
       </c>
       <c r="F16" t="s">
-        <v>20</v>
+        <v>100</v>
       </c>
       <c r="G16" t="s">
-        <v>20</v>
+        <v>119</v>
       </c>
       <c r="H16" t="s">
-        <v>66</v>
+        <v>147</v>
       </c>
       <c r="I16" t="s">
-        <v>20</v>
+        <v>85</v>
       </c>
       <c r="J16" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="K16">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="L16" t="s">
-        <v>20</v>
+        <v>2</v>
       </c>
     </row>
     <row r="17" spans="1:12">
       <c r="A17">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B17" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="C17" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="D17" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E17" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F17" t="s">
-        <v>21</v>
+        <v>101</v>
       </c>
       <c r="G17" t="s">
-        <v>114</v>
+        <v>120</v>
       </c>
       <c r="H17" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="I17" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="J17" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="K17">
         <v>1</v>
@@ -1556,34 +1544,34 @@
     </row>
     <row r="18" spans="1:12">
       <c r="A18">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B18" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="C18" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="D18" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="E18" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="F18" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="G18" t="s">
-        <v>115</v>
+        <v>121</v>
       </c>
       <c r="H18" t="s">
-        <v>145</v>
+        <v>81</v>
       </c>
       <c r="I18" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J18" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="K18">
         <v>1</v>
@@ -1594,34 +1582,34 @@
     </row>
     <row r="19" spans="1:12">
       <c r="A19">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B19" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="C19" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="D19" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="E19" t="s">
         <v>93</v>
       </c>
       <c r="F19" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="G19" t="s">
-        <v>116</v>
+        <v>122</v>
       </c>
       <c r="H19" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="I19" t="s">
-        <v>95</v>
+        <v>156</v>
       </c>
       <c r="J19" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="K19">
         <v>1</v>
@@ -1632,34 +1620,34 @@
     </row>
     <row r="20" spans="1:12">
       <c r="A20">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B20" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="C20" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="D20" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="E20" t="s">
-        <v>87</v>
+        <v>94</v>
       </c>
       <c r="F20" t="s">
-        <v>102</v>
+        <v>13</v>
       </c>
       <c r="G20" t="s">
-        <v>117</v>
+        <v>26</v>
       </c>
       <c r="H20" t="s">
-        <v>140</v>
+        <v>78</v>
       </c>
       <c r="I20" t="s">
-        <v>164</v>
+        <v>94</v>
       </c>
       <c r="J20" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="K20">
         <v>1</v>
@@ -1670,34 +1658,34 @@
     </row>
     <row r="21" spans="1:12">
       <c r="A21">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B21" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="C21" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="D21" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="E21" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="F21" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="G21" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="H21" t="s">
-        <v>78</v>
+        <v>149</v>
       </c>
       <c r="I21" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="J21" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="K21">
         <v>1</v>
@@ -1708,34 +1696,34 @@
     </row>
     <row r="22" spans="1:12">
       <c r="A22">
-        <v>21</v>
+        <v>34</v>
       </c>
       <c r="B22" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C22" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="D22" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="E22" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="F22" t="s">
-        <v>104</v>
+        <v>12</v>
       </c>
       <c r="G22" t="s">
-        <v>119</v>
+        <v>23</v>
       </c>
       <c r="H22" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="I22" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="J22" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="K22">
         <v>1</v>
@@ -1746,34 +1734,34 @@
     </row>
     <row r="23" spans="1:12">
       <c r="A23">
-        <v>22</v>
+        <v>35</v>
       </c>
       <c r="B23" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C23" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="D23" t="s">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="E23" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="F23" t="s">
-        <v>22</v>
+        <v>99</v>
       </c>
       <c r="G23" t="s">
-        <v>58</v>
+        <v>124</v>
       </c>
       <c r="H23" t="s">
-        <v>76</v>
+        <v>150</v>
       </c>
       <c r="I23" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="J23" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="K23">
         <v>1</v>
@@ -1784,34 +1772,34 @@
     </row>
     <row r="24" spans="1:12">
       <c r="A24">
-        <v>23</v>
+        <v>36</v>
       </c>
       <c r="B24" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C24" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="D24" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="E24" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="F24" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="G24" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="H24" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="I24" t="s">
-        <v>95</v>
+        <v>156</v>
       </c>
       <c r="J24" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="K24">
         <v>1</v>
@@ -1822,414 +1810,414 @@
     </row>
     <row r="25" spans="1:12">
       <c r="A25">
-        <v>24</v>
+        <v>37</v>
       </c>
       <c r="B25" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C25" t="s">
-        <v>20</v>
+        <v>46</v>
       </c>
       <c r="D25" t="s">
-        <v>66</v>
+        <v>73</v>
       </c>
       <c r="E25" t="s">
-        <v>20</v>
+        <v>96</v>
       </c>
       <c r="F25" t="s">
-        <v>20</v>
+        <v>101</v>
       </c>
       <c r="G25" t="s">
-        <v>20</v>
+        <v>126</v>
       </c>
       <c r="H25" t="s">
-        <v>66</v>
+        <v>148</v>
       </c>
       <c r="I25" t="s">
-        <v>20</v>
+        <v>86</v>
       </c>
       <c r="J25" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="K25">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L25" t="s">
-        <v>20</v>
+        <v>2</v>
       </c>
     </row>
     <row r="26" spans="1:12">
       <c r="A26">
-        <v>25</v>
+        <v>38</v>
       </c>
       <c r="B26" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C26" t="s">
-        <v>20</v>
+        <v>47</v>
       </c>
       <c r="D26" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="E26" t="s">
-        <v>20</v>
+        <v>94</v>
       </c>
       <c r="F26" t="s">
-        <v>20</v>
+        <v>102</v>
       </c>
       <c r="G26" t="s">
-        <v>20</v>
+        <v>127</v>
       </c>
       <c r="H26" t="s">
-        <v>66</v>
+        <v>137</v>
       </c>
       <c r="I26" t="s">
-        <v>20</v>
+        <v>98</v>
       </c>
       <c r="J26" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="K26">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L26" t="s">
-        <v>20</v>
+        <v>2</v>
       </c>
     </row>
     <row r="27" spans="1:12">
       <c r="A27">
-        <v>26</v>
+        <v>39</v>
       </c>
       <c r="B27" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C27" t="s">
-        <v>20</v>
+        <v>48</v>
       </c>
       <c r="D27" t="s">
-        <v>66</v>
+        <v>77</v>
       </c>
       <c r="E27" t="s">
-        <v>20</v>
+        <v>97</v>
       </c>
       <c r="F27" t="s">
-        <v>20</v>
+        <v>103</v>
       </c>
       <c r="G27" t="s">
-        <v>20</v>
+        <v>128</v>
       </c>
       <c r="H27" t="s">
-        <v>66</v>
+        <v>152</v>
       </c>
       <c r="I27" t="s">
-        <v>20</v>
+        <v>164</v>
       </c>
       <c r="J27" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="K27">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L27" t="s">
-        <v>20</v>
+        <v>2</v>
       </c>
     </row>
     <row r="28" spans="1:12">
       <c r="A28">
-        <v>27</v>
+        <v>40</v>
       </c>
       <c r="B28" t="s">
         <v>20</v>
       </c>
       <c r="C28" t="s">
-        <v>20</v>
+        <v>49</v>
       </c>
       <c r="D28" t="s">
-        <v>66</v>
+        <v>78</v>
       </c>
       <c r="E28" t="s">
-        <v>20</v>
+        <v>86</v>
       </c>
       <c r="F28" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="G28" t="s">
-        <v>20</v>
+        <v>129</v>
       </c>
       <c r="H28" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="I28" t="s">
-        <v>20</v>
+        <v>85</v>
       </c>
       <c r="J28" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="K28">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L28" t="s">
-        <v>20</v>
+        <v>2</v>
       </c>
     </row>
     <row r="29" spans="1:12">
       <c r="A29">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="B29" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C29" t="s">
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="D29" t="s">
-        <v>66</v>
+        <v>79</v>
       </c>
       <c r="E29" t="s">
-        <v>20</v>
+        <v>95</v>
       </c>
       <c r="F29" t="s">
-        <v>20</v>
+        <v>104</v>
       </c>
       <c r="G29" t="s">
-        <v>20</v>
+        <v>130</v>
       </c>
       <c r="H29" t="s">
-        <v>66</v>
+        <v>153</v>
       </c>
       <c r="I29" t="s">
-        <v>20</v>
+        <v>165</v>
       </c>
       <c r="J29" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="K29">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="L29" t="s">
-        <v>20</v>
+        <v>2</v>
       </c>
     </row>
     <row r="30" spans="1:12">
       <c r="A30">
-        <v>29</v>
+        <v>49</v>
       </c>
       <c r="B30" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="C30" t="s">
-        <v>20</v>
+        <v>51</v>
       </c>
       <c r="D30" t="s">
-        <v>66</v>
+        <v>80</v>
       </c>
       <c r="E30" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="F30" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="G30" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="H30" t="s">
-        <v>66</v>
+        <v>80</v>
       </c>
       <c r="I30" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="J30" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="K30">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="L30" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="31" spans="1:12">
       <c r="A31">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="B31" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="C31" t="s">
-        <v>20</v>
+        <v>52</v>
       </c>
       <c r="D31" t="s">
-        <v>66</v>
+        <v>81</v>
       </c>
       <c r="E31" t="s">
-        <v>20</v>
+        <v>98</v>
       </c>
       <c r="F31" t="s">
-        <v>20</v>
+        <v>99</v>
       </c>
       <c r="G31" t="s">
-        <v>20</v>
+        <v>131</v>
       </c>
       <c r="H31" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="I31" t="s">
-        <v>20</v>
+        <v>94</v>
       </c>
       <c r="J31" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="K31">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="L31" t="s">
-        <v>20</v>
+        <v>6</v>
       </c>
     </row>
     <row r="32" spans="1:12">
       <c r="A32">
-        <v>31</v>
+        <v>51</v>
       </c>
       <c r="B32" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C32" t="s">
-        <v>20</v>
+        <v>53</v>
       </c>
       <c r="D32" t="s">
-        <v>66</v>
+        <v>82</v>
       </c>
       <c r="E32" t="s">
-        <v>20</v>
+        <v>89</v>
       </c>
       <c r="F32" t="s">
-        <v>20</v>
+        <v>100</v>
       </c>
       <c r="G32" t="s">
-        <v>20</v>
+        <v>132</v>
       </c>
       <c r="H32" t="s">
-        <v>66</v>
+        <v>154</v>
       </c>
       <c r="I32" t="s">
-        <v>20</v>
+        <v>156</v>
       </c>
       <c r="J32" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="K32">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="L32" t="s">
-        <v>20</v>
+        <v>2</v>
       </c>
     </row>
     <row r="33" spans="1:12">
       <c r="A33">
-        <v>32</v>
+        <v>52</v>
       </c>
       <c r="B33" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C33" t="s">
-        <v>20</v>
+        <v>54</v>
       </c>
       <c r="D33" t="s">
-        <v>66</v>
+        <v>83</v>
       </c>
       <c r="E33" t="s">
-        <v>20</v>
+        <v>90</v>
       </c>
       <c r="F33" t="s">
-        <v>20</v>
+        <v>101</v>
       </c>
       <c r="G33" t="s">
-        <v>20</v>
+        <v>133</v>
       </c>
       <c r="H33" t="s">
-        <v>66</v>
+        <v>155</v>
       </c>
       <c r="I33" t="s">
-        <v>20</v>
+        <v>87</v>
       </c>
       <c r="J33" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="K33">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="L33" t="s">
-        <v>20</v>
+        <v>2</v>
       </c>
     </row>
     <row r="34" spans="1:12">
       <c r="A34">
-        <v>33</v>
+        <v>53</v>
       </c>
       <c r="B34" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C34" t="s">
-        <v>20</v>
+        <v>55</v>
       </c>
       <c r="D34" t="s">
-        <v>66</v>
+        <v>84</v>
       </c>
       <c r="E34" t="s">
-        <v>20</v>
+        <v>85</v>
       </c>
       <c r="F34" t="s">
-        <v>20</v>
+        <v>102</v>
       </c>
       <c r="G34" t="s">
-        <v>20</v>
+        <v>134</v>
       </c>
       <c r="H34" t="s">
-        <v>66</v>
+        <v>84</v>
       </c>
       <c r="I34" t="s">
-        <v>20</v>
+        <v>85</v>
       </c>
       <c r="J34" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="K34">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="L34" t="s">
-        <v>20</v>
+        <v>2</v>
       </c>
     </row>
     <row r="35" spans="1:12">
       <c r="A35">
-        <v>34</v>
+        <v>54</v>
       </c>
       <c r="B35" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="C35" t="s">
-        <v>39</v>
+        <v>56</v>
       </c>
       <c r="D35" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
       <c r="E35" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="F35" t="s">
-        <v>21</v>
+        <v>103</v>
       </c>
       <c r="G35" t="s">
-        <v>121</v>
+        <v>135</v>
       </c>
       <c r="H35" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="I35" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="J35" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="K35">
         <v>1</v>
@@ -2240,72 +2228,72 @@
     </row>
     <row r="36" spans="1:12">
       <c r="A36">
-        <v>35</v>
+        <v>55</v>
       </c>
       <c r="B36" t="s">
+        <v>20</v>
+      </c>
+      <c r="C36" t="s">
+        <v>57</v>
+      </c>
+      <c r="D36" t="s">
+        <v>59</v>
+      </c>
+      <c r="E36" t="s">
+        <v>91</v>
+      </c>
+      <c r="F36" t="s">
         <v>13</v>
       </c>
-      <c r="C36" t="s">
-        <v>40</v>
-      </c>
-      <c r="D36" t="s">
-        <v>73</v>
-      </c>
-      <c r="E36" t="s">
-        <v>95</v>
-      </c>
-      <c r="F36" t="s">
-        <v>100</v>
-      </c>
       <c r="G36" t="s">
-        <v>122</v>
+        <v>24</v>
       </c>
       <c r="H36" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="I36" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="J36" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="K36">
         <v>1</v>
       </c>
       <c r="L36" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="37" spans="1:12">
       <c r="A37">
-        <v>36</v>
+        <v>56</v>
       </c>
       <c r="B37" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="C37" t="s">
-        <v>41</v>
+        <v>58</v>
       </c>
       <c r="D37" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="E37" t="s">
-        <v>89</v>
+        <v>96</v>
       </c>
       <c r="F37" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="G37" t="s">
-        <v>123</v>
+        <v>136</v>
       </c>
       <c r="H37" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="I37" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="J37" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="K37">
         <v>1</v>
@@ -2316,1180 +2304,1180 @@
     </row>
     <row r="38" spans="1:12">
       <c r="A38">
-        <v>37</v>
+        <v>9</v>
       </c>
       <c r="B38" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="C38" t="s">
-        <v>42</v>
+        <v>22</v>
       </c>
       <c r="D38" t="s">
-        <v>71</v>
+        <v>80</v>
       </c>
       <c r="E38" t="s">
-        <v>96</v>
+        <v>22</v>
       </c>
       <c r="F38" t="s">
-        <v>102</v>
+        <v>22</v>
       </c>
       <c r="G38" t="s">
-        <v>124</v>
+        <v>22</v>
       </c>
       <c r="H38" t="s">
-        <v>147</v>
+        <v>80</v>
       </c>
       <c r="I38" t="s">
-        <v>86</v>
+        <v>22</v>
       </c>
       <c r="J38" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
       <c r="K38">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L38" t="s">
-        <v>2</v>
+        <v>22</v>
       </c>
     </row>
     <row r="39" spans="1:12">
       <c r="A39">
-        <v>38</v>
+        <v>10</v>
       </c>
       <c r="B39" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="C39" t="s">
-        <v>43</v>
+        <v>22</v>
       </c>
       <c r="D39" t="s">
-        <v>64</v>
+        <v>80</v>
       </c>
       <c r="E39" t="s">
-        <v>93</v>
+        <v>22</v>
       </c>
       <c r="F39" t="s">
-        <v>103</v>
+        <v>22</v>
       </c>
       <c r="G39" t="s">
-        <v>125</v>
+        <v>22</v>
       </c>
       <c r="H39" t="s">
-        <v>142</v>
+        <v>80</v>
       </c>
       <c r="I39" t="s">
-        <v>99</v>
+        <v>22</v>
       </c>
       <c r="J39" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
       <c r="K39">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L39" t="s">
-        <v>2</v>
+        <v>22</v>
       </c>
     </row>
     <row r="40" spans="1:12">
       <c r="A40">
-        <v>39</v>
+        <v>11</v>
       </c>
       <c r="B40" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="C40" t="s">
-        <v>44</v>
+        <v>22</v>
       </c>
       <c r="D40" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="E40" t="s">
-        <v>97</v>
+        <v>22</v>
       </c>
       <c r="F40" t="s">
-        <v>104</v>
+        <v>22</v>
       </c>
       <c r="G40" t="s">
-        <v>126</v>
+        <v>22</v>
       </c>
       <c r="H40" t="s">
-        <v>151</v>
+        <v>80</v>
       </c>
       <c r="I40" t="s">
-        <v>166</v>
+        <v>22</v>
       </c>
       <c r="J40" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
       <c r="K40">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L40" t="s">
-        <v>2</v>
+        <v>22</v>
       </c>
     </row>
     <row r="41" spans="1:12">
       <c r="A41">
-        <v>40</v>
+        <v>12</v>
       </c>
       <c r="B41" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="C41" t="s">
-        <v>45</v>
+        <v>22</v>
       </c>
       <c r="D41" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="E41" t="s">
-        <v>86</v>
+        <v>22</v>
       </c>
       <c r="F41" t="s">
         <v>22</v>
       </c>
       <c r="G41" t="s">
-        <v>127</v>
+        <v>22</v>
       </c>
       <c r="H41" t="s">
-        <v>60</v>
+        <v>80</v>
       </c>
       <c r="I41" t="s">
-        <v>95</v>
+        <v>22</v>
       </c>
       <c r="J41" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
       <c r="K41">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L41" t="s">
-        <v>2</v>
+        <v>22</v>
       </c>
     </row>
     <row r="42" spans="1:12">
       <c r="A42">
-        <v>41</v>
+        <v>24</v>
       </c>
       <c r="B42" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C42" t="s">
-        <v>46</v>
+        <v>22</v>
       </c>
       <c r="D42" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="E42" t="s">
-        <v>98</v>
+        <v>22</v>
       </c>
       <c r="F42" t="s">
-        <v>105</v>
+        <v>22</v>
       </c>
       <c r="G42" t="s">
-        <v>128</v>
+        <v>22</v>
       </c>
       <c r="H42" t="s">
-        <v>152</v>
+        <v>80</v>
       </c>
       <c r="I42" t="s">
-        <v>167</v>
+        <v>22</v>
       </c>
       <c r="J42" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="K42">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L42" t="s">
-        <v>2</v>
+        <v>22</v>
       </c>
     </row>
     <row r="43" spans="1:12">
       <c r="A43">
-        <v>42</v>
+        <v>25</v>
       </c>
       <c r="B43" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C43" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D43" t="s">
-        <v>66</v>
+        <v>80</v>
       </c>
       <c r="E43" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="F43" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="G43" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="H43" t="s">
-        <v>66</v>
+        <v>80</v>
       </c>
       <c r="I43" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="J43" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="K43">
         <v>2</v>
       </c>
       <c r="L43" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="44" spans="1:12">
       <c r="A44">
-        <v>43</v>
+        <v>26</v>
       </c>
       <c r="B44" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C44" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D44" t="s">
-        <v>66</v>
+        <v>80</v>
       </c>
       <c r="E44" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="F44" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="G44" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="H44" t="s">
-        <v>66</v>
+        <v>80</v>
       </c>
       <c r="I44" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="J44" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="K44">
         <v>2</v>
       </c>
       <c r="L44" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="45" spans="1:12">
       <c r="A45">
-        <v>44</v>
+        <v>27</v>
       </c>
       <c r="B45" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C45" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D45" t="s">
-        <v>66</v>
+        <v>80</v>
       </c>
       <c r="E45" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="F45" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="G45" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="H45" t="s">
-        <v>66</v>
+        <v>80</v>
       </c>
       <c r="I45" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="J45" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="K45">
         <v>2</v>
       </c>
       <c r="L45" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="46" spans="1:12">
       <c r="A46">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B46" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C46" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D46" t="s">
-        <v>66</v>
+        <v>80</v>
       </c>
       <c r="E46" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="F46" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="G46" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="H46" t="s">
-        <v>66</v>
+        <v>80</v>
       </c>
       <c r="I46" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="J46" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="K46">
         <v>2</v>
       </c>
       <c r="L46" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="47" spans="1:12">
       <c r="A47">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B47" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C47" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D47" t="s">
-        <v>66</v>
+        <v>80</v>
       </c>
       <c r="E47" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="F47" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="G47" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="H47" t="s">
-        <v>66</v>
+        <v>80</v>
       </c>
       <c r="I47" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="J47" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="K47">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L47" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="48" spans="1:12">
       <c r="A48">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B48" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C48" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D48" t="s">
-        <v>66</v>
+        <v>80</v>
       </c>
       <c r="E48" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="F48" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="G48" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="H48" t="s">
-        <v>66</v>
+        <v>80</v>
       </c>
       <c r="I48" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="J48" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="K48">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L48" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="49" spans="1:12">
       <c r="A49">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B49" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C49" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D49" t="s">
-        <v>66</v>
+        <v>80</v>
       </c>
       <c r="E49" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="F49" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="G49" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="H49" t="s">
-        <v>66</v>
+        <v>80</v>
       </c>
       <c r="I49" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="J49" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="K49">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="L49" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="50" spans="1:12">
       <c r="A50">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="B50" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="C50" t="s">
-        <v>47</v>
+        <v>22</v>
       </c>
       <c r="D50" t="s">
-        <v>59</v>
+        <v>80</v>
       </c>
       <c r="E50" t="s">
-        <v>94</v>
+        <v>22</v>
       </c>
       <c r="F50" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G50" t="s">
-        <v>57</v>
+        <v>22</v>
       </c>
       <c r="H50" t="s">
-        <v>138</v>
+        <v>80</v>
       </c>
       <c r="I50" t="s">
-        <v>168</v>
+        <v>22</v>
       </c>
       <c r="J50" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="K50">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L50" t="s">
-        <v>2</v>
+        <v>22</v>
       </c>
     </row>
     <row r="51" spans="1:12">
       <c r="A51">
-        <v>50</v>
+        <v>58</v>
       </c>
       <c r="B51" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="C51" t="s">
-        <v>48</v>
+        <v>22</v>
       </c>
       <c r="D51" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="E51" t="s">
-        <v>99</v>
+        <v>22</v>
       </c>
       <c r="F51" t="s">
-        <v>100</v>
+        <v>22</v>
       </c>
       <c r="G51" t="s">
-        <v>129</v>
+        <v>22</v>
       </c>
       <c r="H51" t="s">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="I51" t="s">
-        <v>93</v>
+        <v>22</v>
       </c>
       <c r="J51" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="K51">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L51" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
     </row>
     <row r="52" spans="1:12">
       <c r="A52">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="B52" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="C52" t="s">
-        <v>49</v>
+        <v>22</v>
       </c>
       <c r="D52" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="E52" t="s">
-        <v>87</v>
+        <v>22</v>
       </c>
       <c r="F52" t="s">
-        <v>101</v>
+        <v>22</v>
       </c>
       <c r="G52" t="s">
-        <v>130</v>
+        <v>22</v>
       </c>
       <c r="H52" t="s">
-        <v>153</v>
+        <v>80</v>
       </c>
       <c r="I52" t="s">
-        <v>161</v>
+        <v>22</v>
       </c>
       <c r="J52" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="K52">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L52" t="s">
-        <v>2</v>
+        <v>22</v>
       </c>
     </row>
     <row r="53" spans="1:12">
       <c r="A53">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="B53" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="C53" t="s">
-        <v>50</v>
+        <v>22</v>
       </c>
       <c r="D53" t="s">
         <v>80</v>
       </c>
       <c r="E53" t="s">
-        <v>88</v>
+        <v>22</v>
       </c>
       <c r="F53" t="s">
-        <v>102</v>
+        <v>22</v>
       </c>
       <c r="G53" t="s">
-        <v>131</v>
+        <v>22</v>
       </c>
       <c r="H53" t="s">
-        <v>154</v>
+        <v>80</v>
       </c>
       <c r="I53" t="s">
-        <v>92</v>
+        <v>22</v>
       </c>
       <c r="J53" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="K53">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L53" t="s">
-        <v>2</v>
+        <v>22</v>
       </c>
     </row>
     <row r="54" spans="1:12">
       <c r="A54">
-        <v>53</v>
+        <v>13</v>
       </c>
       <c r="B54" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="C54" t="s">
-        <v>51</v>
+        <v>22</v>
       </c>
       <c r="D54" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E54" t="s">
-        <v>95</v>
+        <v>22</v>
       </c>
       <c r="F54" t="s">
-        <v>103</v>
+        <v>22</v>
       </c>
       <c r="G54" t="s">
-        <v>132</v>
+        <v>22</v>
       </c>
       <c r="H54" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I54" t="s">
-        <v>95</v>
+        <v>22</v>
       </c>
       <c r="J54" t="s">
-        <v>175</v>
+        <v>167</v>
       </c>
       <c r="K54">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="L54" t="s">
-        <v>2</v>
+        <v>22</v>
       </c>
     </row>
     <row r="55" spans="1:12">
       <c r="A55">
-        <v>54</v>
+        <v>14</v>
       </c>
       <c r="B55" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="C55" t="s">
-        <v>52</v>
+        <v>22</v>
       </c>
       <c r="D55" t="s">
-        <v>62</v>
+        <v>80</v>
       </c>
       <c r="E55" t="s">
-        <v>97</v>
+        <v>22</v>
       </c>
       <c r="F55" t="s">
-        <v>104</v>
+        <v>22</v>
       </c>
       <c r="G55" t="s">
-        <v>133</v>
+        <v>22</v>
       </c>
       <c r="H55" t="s">
-        <v>140</v>
+        <v>80</v>
       </c>
       <c r="I55" t="s">
-        <v>162</v>
+        <v>22</v>
       </c>
       <c r="J55" t="s">
-        <v>175</v>
+        <v>167</v>
       </c>
       <c r="K55">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="L55" t="s">
-        <v>2</v>
+        <v>22</v>
       </c>
     </row>
     <row r="56" spans="1:12">
       <c r="A56">
-        <v>55</v>
+        <v>28</v>
       </c>
       <c r="B56" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="C56" t="s">
-        <v>53</v>
+        <v>22</v>
       </c>
       <c r="D56" t="s">
-        <v>64</v>
+        <v>80</v>
       </c>
       <c r="E56" t="s">
-        <v>89</v>
+        <v>22</v>
       </c>
       <c r="F56" t="s">
         <v>22</v>
       </c>
       <c r="G56" t="s">
-        <v>56</v>
+        <v>22</v>
       </c>
       <c r="H56" t="s">
-        <v>142</v>
+        <v>80</v>
       </c>
       <c r="I56" t="s">
-        <v>86</v>
+        <v>22</v>
       </c>
       <c r="J56" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="K56">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="L56" t="s">
-        <v>2</v>
+        <v>22</v>
       </c>
     </row>
     <row r="57" spans="1:12">
       <c r="A57">
-        <v>56</v>
+        <v>29</v>
       </c>
       <c r="B57" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C57" t="s">
-        <v>54</v>
+        <v>22</v>
       </c>
       <c r="D57" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="E57" t="s">
-        <v>96</v>
+        <v>22</v>
       </c>
       <c r="F57" t="s">
-        <v>105</v>
+        <v>22</v>
       </c>
       <c r="G57" t="s">
-        <v>134</v>
+        <v>22</v>
       </c>
       <c r="H57" t="s">
-        <v>152</v>
+        <v>80</v>
       </c>
       <c r="I57" t="s">
-        <v>169</v>
+        <v>22</v>
       </c>
       <c r="J57" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="K57">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="L57" t="s">
-        <v>2</v>
+        <v>22</v>
       </c>
     </row>
     <row r="58" spans="1:12">
       <c r="A58">
-        <v>57</v>
+        <v>46</v>
       </c>
       <c r="B58" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C58" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D58" t="s">
-        <v>66</v>
+        <v>80</v>
       </c>
       <c r="E58" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="F58" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="G58" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="H58" t="s">
-        <v>66</v>
+        <v>80</v>
       </c>
       <c r="I58" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="J58" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="K58">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L58" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="59" spans="1:12">
       <c r="A59">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="B59" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C59" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D59" t="s">
-        <v>66</v>
+        <v>80</v>
       </c>
       <c r="E59" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="F59" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="G59" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="H59" t="s">
-        <v>66</v>
+        <v>80</v>
       </c>
       <c r="I59" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="J59" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="K59">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L59" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="60" spans="1:12">
       <c r="A60">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B60" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C60" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D60" t="s">
-        <v>66</v>
+        <v>80</v>
       </c>
       <c r="E60" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="F60" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="G60" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="H60" t="s">
-        <v>66</v>
+        <v>80</v>
       </c>
       <c r="I60" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="J60" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="K60">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L60" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="61" spans="1:12">
       <c r="A61">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B61" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C61" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D61" t="s">
-        <v>66</v>
+        <v>80</v>
       </c>
       <c r="E61" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="F61" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="G61" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="H61" t="s">
-        <v>66</v>
+        <v>80</v>
       </c>
       <c r="I61" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="J61" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="K61">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L61" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="62" spans="1:12">
       <c r="A62">
-        <v>61</v>
+        <v>15</v>
       </c>
       <c r="B62" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C62" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D62" t="s">
-        <v>66</v>
+        <v>80</v>
       </c>
       <c r="E62" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="F62" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="G62" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="H62" t="s">
-        <v>66</v>
+        <v>80</v>
       </c>
       <c r="I62" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="J62" t="s">
-        <v>175</v>
+        <v>167</v>
       </c>
       <c r="K62">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="L62" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="63" spans="1:12">
       <c r="A63">
-        <v>62</v>
+        <v>30</v>
       </c>
       <c r="B63" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C63" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D63" t="s">
-        <v>66</v>
+        <v>80</v>
       </c>
       <c r="E63" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="F63" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="G63" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="H63" t="s">
-        <v>66</v>
+        <v>80</v>
       </c>
       <c r="I63" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="J63" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="K63">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="L63" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="64" spans="1:12">
       <c r="A64">
-        <v>63</v>
+        <v>48</v>
       </c>
       <c r="B64" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C64" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D64" t="s">
-        <v>66</v>
+        <v>80</v>
       </c>
       <c r="E64" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="F64" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="G64" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="H64" t="s">
-        <v>66</v>
+        <v>80</v>
       </c>
       <c r="I64" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="J64" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="K64">
         <v>4</v>
       </c>
       <c r="L64" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="65" spans="1:12">
       <c r="A65">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B65" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C65" t="s">
-        <v>55</v>
+        <v>22</v>
       </c>
       <c r="D65" t="s">
-        <v>64</v>
+        <v>80</v>
       </c>
       <c r="E65" t="s">
-        <v>95</v>
+        <v>22</v>
       </c>
       <c r="F65" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G65" t="s">
-        <v>121</v>
+        <v>22</v>
       </c>
       <c r="H65" t="s">
-        <v>142</v>
+        <v>80</v>
       </c>
       <c r="I65" t="s">
-        <v>161</v>
+        <v>22</v>
       </c>
       <c r="J65" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="K65">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="L65" t="s">
-        <v>2</v>
+        <v>22</v>
       </c>
     </row>
     <row r="66" spans="1:12">
       <c r="A66">
-        <v>65</v>
+        <v>31</v>
       </c>
       <c r="B66" t="s">
         <v>22</v>
       </c>
       <c r="C66" t="s">
-        <v>56</v>
+        <v>22</v>
       </c>
       <c r="D66" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E66" t="s">
-        <v>95</v>
+        <v>22</v>
       </c>
       <c r="F66" t="s">
         <v>22</v>
       </c>
       <c r="G66" t="s">
-        <v>135</v>
+        <v>22</v>
       </c>
       <c r="H66" t="s">
-        <v>155</v>
+        <v>80</v>
       </c>
       <c r="I66" t="s">
-        <v>160</v>
+        <v>22</v>
       </c>
       <c r="J66" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="K66">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="L66" t="s">
-        <v>2</v>
+        <v>22</v>
       </c>
     </row>
     <row r="67" spans="1:12">
       <c r="A67">
-        <v>66</v>
+        <v>33</v>
       </c>
       <c r="B67" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C67" t="s">
-        <v>57</v>
+        <v>22</v>
       </c>
       <c r="D67" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="E67" t="s">
-        <v>86</v>
+        <v>22</v>
       </c>
       <c r="F67" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G67" t="s">
-        <v>136</v>
+        <v>22</v>
       </c>
       <c r="H67" t="s">
-        <v>156</v>
+        <v>80</v>
       </c>
       <c r="I67" t="s">
-        <v>92</v>
+        <v>22</v>
       </c>
       <c r="J67" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="K67">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="L67" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
     </row>
     <row r="68" spans="1:12">
       <c r="A68">
-        <v>67</v>
+        <v>32</v>
       </c>
       <c r="B68" t="s">
         <v>22</v>
       </c>
       <c r="C68" t="s">
-        <v>58</v>
+        <v>22</v>
       </c>
       <c r="D68" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="E68" t="s">
-        <v>92</v>
+        <v>22</v>
       </c>
       <c r="F68" t="s">
         <v>22</v>
       </c>
       <c r="G68" t="s">
-        <v>137</v>
+        <v>22</v>
       </c>
       <c r="H68" t="s">
-        <v>157</v>
+        <v>80</v>
       </c>
       <c r="I68" t="s">
-        <v>86</v>
+        <v>22</v>
       </c>
       <c r="J68" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="K68">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="L68" t="s">
-        <v>2</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
seeds now get promoted too
</commit_message>
<xml_diff>
--- a/predict.xlsx
+++ b/predict.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="682" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="682" uniqueCount="197">
   <si>
     <t>Index</t>
   </si>
@@ -82,9 +82,6 @@
     <t>02</t>
   </si>
   <si>
-    <t>?</t>
-  </si>
-  <si>
     <t>Howard</t>
   </si>
   <si>
@@ -97,36 +94,39 @@
     <t>Colorado</t>
   </si>
   <si>
+    <t>Connecticut</t>
+  </si>
+  <si>
+    <t>Florida Atlantic</t>
+  </si>
+  <si>
+    <t>San Diego St.</t>
+  </si>
+  <si>
+    <t>Auburn</t>
+  </si>
+  <si>
+    <t>BYU</t>
+  </si>
+  <si>
+    <t>Illinois</t>
+  </si>
+  <si>
+    <t>Washington St.</t>
+  </si>
+  <si>
+    <t>Iowa St.</t>
+  </si>
+  <si>
+    <t>Houston</t>
+  </si>
+  <si>
+    <t>Nebraska</t>
+  </si>
+  <si>
     <t>Wisconsin</t>
   </si>
   <si>
-    <t>FIU</t>
-  </si>
-  <si>
-    <t>San Diego St.</t>
-  </si>
-  <si>
-    <t>Auburn</t>
-  </si>
-  <si>
-    <t>BYU</t>
-  </si>
-  <si>
-    <t>Illinois</t>
-  </si>
-  <si>
-    <t>Washington St.</t>
-  </si>
-  <si>
-    <t>Iowa St.</t>
-  </si>
-  <si>
-    <t>Houston</t>
-  </si>
-  <si>
-    <t>Nebraska</t>
-  </si>
-  <si>
     <t>Duke</t>
   </si>
   <si>
@@ -202,21 +202,24 @@
     <t>57%</t>
   </si>
   <si>
+    <t>99%</t>
+  </si>
+  <si>
+    <t>48%</t>
+  </si>
+  <si>
+    <t>78%</t>
+  </si>
+  <si>
+    <t>88%</t>
+  </si>
+  <si>
+    <t>75%</t>
+  </si>
+  <si>
     <t>93%</t>
   </si>
   <si>
-    <t>6%</t>
-  </si>
-  <si>
-    <t>78%</t>
-  </si>
-  <si>
-    <t>88%</t>
-  </si>
-  <si>
-    <t>75%</t>
-  </si>
-  <si>
     <t>97%</t>
   </si>
   <si>
@@ -232,15 +235,9 @@
     <t>84%</t>
   </si>
   <si>
-    <t>48%</t>
-  </si>
-  <si>
     <t>91%</t>
   </si>
   <si>
-    <t>99%</t>
-  </si>
-  <si>
     <t>42%</t>
   </si>
   <si>
@@ -268,322 +265,322 @@
     <t>50%</t>
   </si>
   <si>
+    <t>30%</t>
+  </si>
+  <si>
+    <t>39%</t>
+  </si>
+  <si>
+    <t>27%</t>
+  </si>
+  <si>
+    <t>79%</t>
+  </si>
+  <si>
+    <t>35%</t>
+  </si>
+  <si>
+    <t>45%</t>
+  </si>
+  <si>
+    <t>38%</t>
+  </si>
+  <si>
+    <t>64%</t>
+  </si>
+  <si>
+    <t>41%</t>
+  </si>
+  <si>
+    <t>28%</t>
+  </si>
+  <si>
+    <t>82%</t>
+  </si>
+  <si>
+    <t>63%</t>
+  </si>
+  <si>
+    <t>31%</t>
+  </si>
+  <si>
+    <t>58%</t>
+  </si>
+  <si>
+    <t>72%</t>
+  </si>
+  <si>
+    <t>69%</t>
+  </si>
+  <si>
+    <t>49%</t>
+  </si>
+  <si>
+    <t>60%</t>
+  </si>
+  <si>
+    <t>73%</t>
+  </si>
+  <si>
+    <t>65</t>
+  </si>
+  <si>
+    <t>66</t>
+  </si>
+  <si>
+    <t>68</t>
+  </si>
+  <si>
+    <t>79</t>
+  </si>
+  <si>
+    <t>71</t>
+  </si>
+  <si>
+    <t>74</t>
+  </si>
+  <si>
+    <t>67</t>
+  </si>
+  <si>
+    <t>76</t>
+  </si>
+  <si>
+    <t>75</t>
+  </si>
+  <si>
+    <t>70</t>
+  </si>
+  <si>
+    <t>81</t>
+  </si>
+  <si>
+    <t>77</t>
+  </si>
+  <si>
+    <t>73</t>
+  </si>
+  <si>
+    <t>80</t>
+  </si>
+  <si>
+    <t>69</t>
+  </si>
+  <si>
+    <t>63</t>
+  </si>
+  <si>
+    <t>64</t>
+  </si>
+  <si>
+    <t>62</t>
+  </si>
+  <si>
+    <t>72</t>
+  </si>
+  <si>
+    <t>09</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>Wagner</t>
+  </si>
+  <si>
+    <t>Virginia</t>
+  </si>
+  <si>
+    <t>Montana St.</t>
+  </si>
+  <si>
+    <t>Boise St.</t>
+  </si>
+  <si>
+    <t>Stetson</t>
+  </si>
+  <si>
+    <t>Northwestern</t>
+  </si>
+  <si>
+    <t>UAB</t>
+  </si>
+  <si>
+    <t>Yale</t>
+  </si>
+  <si>
+    <t>Duquesne</t>
+  </si>
+  <si>
+    <t>Morehead St.</t>
+  </si>
+  <si>
+    <t>Drake</t>
+  </si>
+  <si>
+    <t>South Dakota St.</t>
+  </si>
+  <si>
+    <t>Longwood</t>
+  </si>
+  <si>
+    <t>Texas A&amp;M</t>
+  </si>
+  <si>
+    <t>James Madison</t>
+  </si>
+  <si>
+    <t>Vermont</t>
+  </si>
+  <si>
+    <t>N.C. State</t>
+  </si>
+  <si>
+    <t>Oakland</t>
+  </si>
+  <si>
+    <t>Western Kentucky</t>
+  </si>
+  <si>
+    <t>Michigan St.</t>
+  </si>
+  <si>
+    <t>Grand Canyon</t>
+  </si>
+  <si>
+    <t>Charleston</t>
+  </si>
+  <si>
+    <t>New Mexico</t>
+  </si>
+  <si>
+    <t>Colgate</t>
+  </si>
+  <si>
+    <t>Nevada</t>
+  </si>
+  <si>
+    <t>Long Beach St.</t>
+  </si>
+  <si>
+    <t>TCU</t>
+  </si>
+  <si>
+    <t>McNeese St.</t>
+  </si>
+  <si>
+    <t>Samford</t>
+  </si>
+  <si>
+    <t>Oregon</t>
+  </si>
+  <si>
+    <t>Akron</t>
+  </si>
+  <si>
+    <t>Saint Peter's</t>
+  </si>
+  <si>
+    <t>46%</t>
+  </si>
+  <si>
+    <t>56%</t>
+  </si>
+  <si>
+    <t>43%</t>
+  </si>
+  <si>
+    <t>1%</t>
+  </si>
+  <si>
+    <t>22%</t>
+  </si>
+  <si>
+    <t>12%</t>
+  </si>
+  <si>
+    <t>25%</t>
+  </si>
+  <si>
+    <t>7%</t>
+  </si>
+  <si>
+    <t>3%</t>
+  </si>
+  <si>
+    <t>32%</t>
+  </si>
+  <si>
+    <t>16%</t>
+  </si>
+  <si>
+    <t>9%</t>
+  </si>
+  <si>
+    <t>11%</t>
+  </si>
+  <si>
+    <t>4%</t>
+  </si>
+  <si>
+    <t>24%</t>
+  </si>
+  <si>
+    <t>21%</t>
+  </si>
+  <si>
+    <t>65%</t>
+  </si>
+  <si>
+    <t>55%</t>
+  </si>
+  <si>
+    <t>36%</t>
+  </si>
+  <si>
     <t>59%</t>
   </si>
   <si>
-    <t>30%</t>
-  </si>
-  <si>
-    <t>39%</t>
-  </si>
-  <si>
-    <t>27%</t>
-  </si>
-  <si>
-    <t>79%</t>
-  </si>
-  <si>
-    <t>35%</t>
-  </si>
-  <si>
-    <t>45%</t>
-  </si>
-  <si>
-    <t>38%</t>
-  </si>
-  <si>
-    <t>64%</t>
-  </si>
-  <si>
-    <t>41%</t>
-  </si>
-  <si>
-    <t>28%</t>
-  </si>
-  <si>
-    <t>82%</t>
-  </si>
-  <si>
-    <t>63%</t>
-  </si>
-  <si>
-    <t>31%</t>
-  </si>
-  <si>
-    <t>58%</t>
-  </si>
-  <si>
-    <t>69%</t>
-  </si>
-  <si>
-    <t>49%</t>
-  </si>
-  <si>
-    <t>60%</t>
-  </si>
-  <si>
-    <t>65</t>
-  </si>
-  <si>
-    <t>66</t>
-  </si>
-  <si>
-    <t>68</t>
-  </si>
-  <si>
-    <t>74</t>
+    <t>18%</t>
+  </si>
+  <si>
+    <t>37%</t>
+  </si>
+  <si>
+    <t>40%</t>
+  </si>
+  <si>
+    <t>61</t>
+  </si>
+  <si>
+    <t>52</t>
+  </si>
+  <si>
+    <t>60</t>
+  </si>
+  <si>
+    <t>55</t>
+  </si>
+  <si>
+    <t>58</t>
+  </si>
+  <si>
+    <t>57</t>
   </si>
   <si>
     <t>59</t>
-  </si>
-  <si>
-    <t>71</t>
-  </si>
-  <si>
-    <t>67</t>
-  </si>
-  <si>
-    <t>76</t>
-  </si>
-  <si>
-    <t>75</t>
-  </si>
-  <si>
-    <t>70</t>
-  </si>
-  <si>
-    <t>79</t>
-  </si>
-  <si>
-    <t>81</t>
-  </si>
-  <si>
-    <t>77</t>
-  </si>
-  <si>
-    <t>73</t>
-  </si>
-  <si>
-    <t>80</t>
-  </si>
-  <si>
-    <t>69</t>
-  </si>
-  <si>
-    <t>63</t>
-  </si>
-  <si>
-    <t>64</t>
-  </si>
-  <si>
-    <t>62</t>
-  </si>
-  <si>
-    <t>72</t>
-  </si>
-  <si>
-    <t>09</t>
-  </si>
-  <si>
-    <t>12</t>
-  </si>
-  <si>
-    <t>13</t>
-  </si>
-  <si>
-    <t>11</t>
-  </si>
-  <si>
-    <t>14</t>
-  </si>
-  <si>
-    <t>15</t>
-  </si>
-  <si>
-    <t>Wagner</t>
-  </si>
-  <si>
-    <t>Virginia</t>
-  </si>
-  <si>
-    <t>Montana St.</t>
-  </si>
-  <si>
-    <t>Boise St.</t>
-  </si>
-  <si>
-    <t>Stetson</t>
-  </si>
-  <si>
-    <t>Northwestern</t>
-  </si>
-  <si>
-    <t>UAB</t>
-  </si>
-  <si>
-    <t>Yale</t>
-  </si>
-  <si>
-    <t>Duquesne</t>
-  </si>
-  <si>
-    <t>Morehead St.</t>
-  </si>
-  <si>
-    <t>Drake</t>
-  </si>
-  <si>
-    <t>South Dakota St.</t>
-  </si>
-  <si>
-    <t>Longwood</t>
-  </si>
-  <si>
-    <t>Texas A&amp;M</t>
-  </si>
-  <si>
-    <t>James Madison</t>
-  </si>
-  <si>
-    <t>Vermont</t>
-  </si>
-  <si>
-    <t>N.C. State</t>
-  </si>
-  <si>
-    <t>Oakland</t>
-  </si>
-  <si>
-    <t>Western Kentucky</t>
-  </si>
-  <si>
-    <t>Michigan St.</t>
-  </si>
-  <si>
-    <t>Grand Canyon</t>
-  </si>
-  <si>
-    <t>Charleston</t>
-  </si>
-  <si>
-    <t>New Mexico</t>
-  </si>
-  <si>
-    <t>Colgate</t>
-  </si>
-  <si>
-    <t>Nevada</t>
-  </si>
-  <si>
-    <t>Long Beach St.</t>
-  </si>
-  <si>
-    <t>TCU</t>
-  </si>
-  <si>
-    <t>McNeese St.</t>
-  </si>
-  <si>
-    <t>Samford</t>
-  </si>
-  <si>
-    <t>Oregon</t>
-  </si>
-  <si>
-    <t>Akron</t>
-  </si>
-  <si>
-    <t>Saint Peter's</t>
-  </si>
-  <si>
-    <t>46%</t>
-  </si>
-  <si>
-    <t>56%</t>
-  </si>
-  <si>
-    <t>43%</t>
-  </si>
-  <si>
-    <t>7%</t>
-  </si>
-  <si>
-    <t>94%</t>
-  </si>
-  <si>
-    <t>22%</t>
-  </si>
-  <si>
-    <t>12%</t>
-  </si>
-  <si>
-    <t>25%</t>
-  </si>
-  <si>
-    <t>3%</t>
-  </si>
-  <si>
-    <t>32%</t>
-  </si>
-  <si>
-    <t>16%</t>
-  </si>
-  <si>
-    <t>9%</t>
-  </si>
-  <si>
-    <t>1%</t>
-  </si>
-  <si>
-    <t>11%</t>
-  </si>
-  <si>
-    <t>4%</t>
-  </si>
-  <si>
-    <t>24%</t>
-  </si>
-  <si>
-    <t>73%</t>
-  </si>
-  <si>
-    <t>21%</t>
-  </si>
-  <si>
-    <t>65%</t>
-  </si>
-  <si>
-    <t>55%</t>
-  </si>
-  <si>
-    <t>36%</t>
-  </si>
-  <si>
-    <t>72%</t>
-  </si>
-  <si>
-    <t>18%</t>
-  </si>
-  <si>
-    <t>37%</t>
-  </si>
-  <si>
-    <t>40%</t>
-  </si>
-  <si>
-    <t>61</t>
-  </si>
-  <si>
-    <t>58</t>
-  </si>
-  <si>
-    <t>60</t>
-  </si>
-  <si>
-    <t>55</t>
-  </si>
-  <si>
-    <t>57</t>
   </si>
   <si>
     <t>56</t>
@@ -1017,7 +1014,7 @@
         <v>12</v>
       </c>
       <c r="C2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D2" t="s">
         <v>58</v>
@@ -1029,16 +1026,16 @@
         <v>12</v>
       </c>
       <c r="G2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="J2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="K2">
         <v>0</v>
@@ -1055,7 +1052,7 @@
         <v>13</v>
       </c>
       <c r="C3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D3" t="s">
         <v>59</v>
@@ -1067,16 +1064,16 @@
         <v>13</v>
       </c>
       <c r="G3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="H3" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="I3" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="J3" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="K3">
         <v>0</v>
@@ -1093,7 +1090,7 @@
         <v>12</v>
       </c>
       <c r="C4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D4" t="s">
         <v>60</v>
@@ -1105,16 +1102,16 @@
         <v>12</v>
       </c>
       <c r="G4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="H4" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="I4" t="s">
         <v>104</v>
       </c>
       <c r="J4" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="K4">
         <v>0</v>
@@ -1131,7 +1128,7 @@
         <v>13</v>
       </c>
       <c r="C5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D5" t="s">
         <v>61</v>
@@ -1143,16 +1140,16 @@
         <v>13</v>
       </c>
       <c r="G5" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="H5" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="I5" t="s">
         <v>103</v>
       </c>
       <c r="J5" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="K5">
         <v>0</v>
@@ -1169,7 +1166,7 @@
         <v>14</v>
       </c>
       <c r="C6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D6" t="s">
         <v>62</v>
@@ -1181,16 +1178,16 @@
         <v>12</v>
       </c>
       <c r="G6" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="H6" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="I6" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="J6" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="K6">
         <v>1</v>
@@ -1207,34 +1204,34 @@
         <v>15</v>
       </c>
       <c r="C7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D7" t="s">
         <v>63</v>
       </c>
       <c r="E7" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="F7" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G7" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="H7" t="s">
-        <v>164</v>
+        <v>77</v>
       </c>
       <c r="I7" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="J7" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="K7">
         <v>1</v>
       </c>
       <c r="L7" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:12">
@@ -1245,28 +1242,28 @@
         <v>16</v>
       </c>
       <c r="C8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D8" t="s">
         <v>64</v>
       </c>
       <c r="E8" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F8" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G8" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H8" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="I8" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="J8" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="K8">
         <v>1</v>
@@ -1283,28 +1280,28 @@
         <v>17</v>
       </c>
       <c r="C9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D9" t="s">
         <v>65</v>
       </c>
       <c r="E9" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="F9" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G9" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="H9" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="I9" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="J9" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="K9">
         <v>1</v>
@@ -1321,28 +1318,28 @@
         <v>18</v>
       </c>
       <c r="C10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D10" t="s">
         <v>66</v>
       </c>
       <c r="E10" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F10" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G10" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="H10" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="I10" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="J10" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="K10">
         <v>1</v>
@@ -1359,28 +1356,28 @@
         <v>19</v>
       </c>
       <c r="C11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D11" t="s">
         <v>65</v>
       </c>
       <c r="E11" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="F11" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="G11" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="H11" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="I11" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="J11" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="K11">
         <v>1</v>
@@ -1397,7 +1394,7 @@
         <v>20</v>
       </c>
       <c r="C12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D12" t="s">
         <v>58</v>
@@ -1409,16 +1406,16 @@
         <v>13</v>
       </c>
       <c r="G12" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="H12" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I12" t="s">
         <v>103</v>
       </c>
       <c r="J12" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="K12">
         <v>1</v>
@@ -1435,28 +1432,28 @@
         <v>21</v>
       </c>
       <c r="C13" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D13" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="E13" t="s">
         <v>109</v>
       </c>
       <c r="F13" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G13" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="H13" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="I13" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="J13" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="K13">
         <v>1</v>
@@ -1473,10 +1470,10 @@
         <v>14</v>
       </c>
       <c r="C14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D14" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E14" t="s">
         <v>110</v>
@@ -1485,16 +1482,16 @@
         <v>12</v>
       </c>
       <c r="G14" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="H14" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="I14" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="J14" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="K14">
         <v>1</v>
@@ -1511,28 +1508,28 @@
         <v>15</v>
       </c>
       <c r="C15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D15" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E15" t="s">
         <v>104</v>
       </c>
       <c r="F15" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G15" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H15" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="I15" t="s">
         <v>104</v>
       </c>
       <c r="J15" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="K15">
         <v>1</v>
@@ -1549,28 +1546,28 @@
         <v>16</v>
       </c>
       <c r="C16" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="D16" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E16" t="s">
         <v>111</v>
       </c>
       <c r="F16" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G16" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="H16" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="I16" t="s">
         <v>102</v>
       </c>
       <c r="J16" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="K16">
         <v>1</v>
@@ -1593,22 +1590,22 @@
         <v>65</v>
       </c>
       <c r="E17" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F17" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G17" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H17" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="I17" t="s">
         <v>186</v>
       </c>
       <c r="J17" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="K17">
         <v>1</v>
@@ -1628,25 +1625,25 @@
         <v>38</v>
       </c>
       <c r="D18" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="E18" t="s">
         <v>104</v>
       </c>
       <c r="F18" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G18" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H18" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I18" t="s">
         <v>108</v>
       </c>
       <c r="J18" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="K18">
         <v>1</v>
@@ -1666,25 +1663,25 @@
         <v>39</v>
       </c>
       <c r="D19" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="E19" t="s">
         <v>110</v>
       </c>
       <c r="F19" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="G19" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="H19" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="I19" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="J19" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="K19">
         <v>1</v>
@@ -1704,7 +1701,7 @@
         <v>40</v>
       </c>
       <c r="D20" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="E20" t="s">
         <v>111</v>
@@ -1713,16 +1710,16 @@
         <v>13</v>
       </c>
       <c r="G20" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H20" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="I20" t="s">
         <v>111</v>
       </c>
       <c r="J20" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="K20">
         <v>1</v>
@@ -1745,22 +1742,22 @@
         <v>73</v>
       </c>
       <c r="E21" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="F21" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G21" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="H21" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="I21" t="s">
         <v>102</v>
       </c>
       <c r="J21" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="K21">
         <v>1</v>
@@ -1780,25 +1777,25 @@
         <v>42</v>
       </c>
       <c r="D22" t="s">
-        <v>74</v>
+        <v>62</v>
       </c>
       <c r="E22" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F22" t="s">
         <v>12</v>
       </c>
       <c r="G22" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H22" t="s">
-        <v>172</v>
+        <v>162</v>
       </c>
       <c r="I22" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="J22" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="K22">
         <v>1</v>
@@ -1818,25 +1815,25 @@
         <v>43</v>
       </c>
       <c r="D23" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E23" t="s">
         <v>102</v>
       </c>
       <c r="F23" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G23" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="H23" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="I23" t="s">
         <v>108</v>
       </c>
       <c r="J23" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="K23">
         <v>1</v>
@@ -1856,25 +1853,25 @@
         <v>44</v>
       </c>
       <c r="D24" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E24" t="s">
         <v>108</v>
       </c>
       <c r="F24" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G24" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="H24" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="I24" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="J24" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="K24">
         <v>1</v>
@@ -1894,25 +1891,25 @@
         <v>45</v>
       </c>
       <c r="D25" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="E25" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F25" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G25" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="H25" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="I25" t="s">
         <v>103</v>
       </c>
       <c r="J25" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="K25">
         <v>1</v>
@@ -1938,19 +1935,19 @@
         <v>111</v>
       </c>
       <c r="F26" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G26" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="H26" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I26" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="J26" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="K26">
         <v>1</v>
@@ -1970,25 +1967,25 @@
         <v>47</v>
       </c>
       <c r="D27" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E27" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F27" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="G27" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="H27" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="I27" t="s">
-        <v>106</v>
+        <v>188</v>
       </c>
       <c r="J27" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="K27">
         <v>1</v>
@@ -2008,7 +2005,7 @@
         <v>48</v>
       </c>
       <c r="D28" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E28" t="s">
         <v>103</v>
@@ -2017,16 +2014,16 @@
         <v>13</v>
       </c>
       <c r="G28" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="H28" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="I28" t="s">
         <v>102</v>
       </c>
       <c r="J28" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="K28">
         <v>1</v>
@@ -2046,25 +2043,25 @@
         <v>49</v>
       </c>
       <c r="D29" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E29" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F29" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G29" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="H29" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="I29" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="J29" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="K29">
         <v>1</v>
@@ -2084,25 +2081,25 @@
         <v>50</v>
       </c>
       <c r="D30" t="s">
-        <v>74</v>
+        <v>62</v>
       </c>
       <c r="E30" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F30" t="s">
         <v>12</v>
       </c>
       <c r="G30" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="H30" t="s">
-        <v>172</v>
+        <v>162</v>
       </c>
       <c r="I30" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="J30" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="K30">
         <v>1</v>
@@ -2122,25 +2119,25 @@
         <v>51</v>
       </c>
       <c r="D31" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E31" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F31" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G31" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="H31" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="I31" t="s">
         <v>111</v>
       </c>
       <c r="J31" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="K31">
         <v>1</v>
@@ -2160,25 +2157,25 @@
         <v>52</v>
       </c>
       <c r="D32" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E32" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F32" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G32" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="H32" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="I32" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="J32" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="K32">
         <v>1</v>
@@ -2198,25 +2195,25 @@
         <v>53</v>
       </c>
       <c r="D33" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E33" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="F33" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G33" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="H33" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="I33" t="s">
         <v>104</v>
       </c>
       <c r="J33" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="K33">
         <v>1</v>
@@ -2236,25 +2233,25 @@
         <v>54</v>
       </c>
       <c r="D34" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E34" t="s">
         <v>102</v>
       </c>
       <c r="F34" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G34" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="H34" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="I34" t="s">
         <v>102</v>
       </c>
       <c r="J34" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="K34">
         <v>1</v>
@@ -2277,22 +2274,22 @@
         <v>65</v>
       </c>
       <c r="E35" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F35" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="G35" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="H35" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="I35" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="J35" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="K35">
         <v>1</v>
@@ -2321,16 +2318,16 @@
         <v>13</v>
       </c>
       <c r="G36" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H36" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I36" t="s">
         <v>103</v>
       </c>
       <c r="J36" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="K36">
         <v>1</v>
@@ -2350,25 +2347,25 @@
         <v>57</v>
       </c>
       <c r="D37" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E37" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F37" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G37" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="H37" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="I37" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="J37" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="K37">
         <v>1</v>
@@ -2382,31 +2379,31 @@
         <v>9</v>
       </c>
       <c r="B38" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="C38" t="s">
+        <v>26</v>
+      </c>
+      <c r="D38" t="s">
+        <v>76</v>
+      </c>
+      <c r="E38" t="s">
+        <v>114</v>
+      </c>
+      <c r="F38" t="s">
+        <v>15</v>
+      </c>
+      <c r="G38" t="s">
         <v>27</v>
       </c>
-      <c r="D38" t="s">
-        <v>84</v>
-      </c>
-      <c r="E38" t="s">
-        <v>103</v>
-      </c>
-      <c r="F38" t="s">
-        <v>22</v>
-      </c>
-      <c r="G38" t="s">
-        <v>133</v>
-      </c>
       <c r="H38" t="s">
-        <v>93</v>
+        <v>171</v>
       </c>
       <c r="I38" t="s">
-        <v>119</v>
+        <v>184</v>
       </c>
       <c r="J38" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="K38">
         <v>2</v>
@@ -2420,31 +2417,31 @@
         <v>10</v>
       </c>
       <c r="B39" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="C39" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D39" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E39" t="s">
         <v>102</v>
       </c>
       <c r="F39" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="G39" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H39" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="I39" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="J39" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="K39">
         <v>2</v>
@@ -2458,31 +2455,31 @@
         <v>11</v>
       </c>
       <c r="B40" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C40" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D40" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E40" t="s">
         <v>104</v>
       </c>
       <c r="F40" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="G40" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H40" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I40" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="J40" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="K40">
         <v>2</v>
@@ -2496,31 +2493,31 @@
         <v>12</v>
       </c>
       <c r="B41" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C41" t="s">
+        <v>32</v>
+      </c>
+      <c r="D41" t="s">
+        <v>85</v>
+      </c>
+      <c r="E41" t="s">
+        <v>117</v>
+      </c>
+      <c r="F41" t="s">
+        <v>21</v>
+      </c>
+      <c r="G41" t="s">
         <v>33</v>
       </c>
-      <c r="D41" t="s">
-        <v>87</v>
-      </c>
-      <c r="E41" t="s">
-        <v>118</v>
-      </c>
-      <c r="F41" t="s">
-        <v>22</v>
-      </c>
-      <c r="G41" t="s">
-        <v>34</v>
-      </c>
       <c r="H41" t="s">
-        <v>176</v>
+        <v>101</v>
       </c>
       <c r="I41" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="J41" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="K41">
         <v>2</v>
@@ -2534,31 +2531,31 @@
         <v>24</v>
       </c>
       <c r="B42" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="C42" t="s">
+        <v>34</v>
+      </c>
+      <c r="D42" t="s">
+        <v>86</v>
+      </c>
+      <c r="E42" t="s">
+        <v>106</v>
+      </c>
+      <c r="F42" t="s">
+        <v>15</v>
+      </c>
+      <c r="G42" t="s">
         <v>35</v>
       </c>
-      <c r="D42" t="s">
-        <v>88</v>
-      </c>
-      <c r="E42" t="s">
-        <v>107</v>
-      </c>
-      <c r="F42" t="s">
-        <v>22</v>
-      </c>
-      <c r="G42" t="s">
-        <v>36</v>
-      </c>
       <c r="H42" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="I42" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="J42" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="K42">
         <v>2</v>
@@ -2572,31 +2569,31 @@
         <v>25</v>
       </c>
       <c r="B43" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="C43" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="D43" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E43" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F43" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="G43" t="s">
         <v>37</v>
       </c>
       <c r="H43" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="I43" t="s">
         <v>104</v>
       </c>
       <c r="J43" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="K43">
         <v>2</v>
@@ -2610,31 +2607,31 @@
         <v>26</v>
       </c>
       <c r="B44" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C44" t="s">
         <v>38</v>
       </c>
       <c r="D44" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E44" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F44" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="G44" t="s">
         <v>39</v>
       </c>
       <c r="H44" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="I44" t="s">
         <v>111</v>
       </c>
       <c r="J44" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="K44">
         <v>2</v>
@@ -2648,19 +2645,19 @@
         <v>27</v>
       </c>
       <c r="B45" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C45" t="s">
         <v>40</v>
       </c>
       <c r="D45" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E45" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F45" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G45" t="s">
         <v>41</v>
@@ -2669,10 +2666,10 @@
         <v>59</v>
       </c>
       <c r="I45" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="J45" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="K45">
         <v>2</v>
@@ -2686,31 +2683,31 @@
         <v>42</v>
       </c>
       <c r="B46" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="C46" t="s">
         <v>42</v>
       </c>
       <c r="D46" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E46" t="s">
         <v>111</v>
       </c>
       <c r="F46" t="s">
-        <v>22</v>
+        <v>121</v>
       </c>
       <c r="G46" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="H46" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="I46" t="s">
         <v>103</v>
       </c>
       <c r="J46" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="K46">
         <v>2</v>
@@ -2724,31 +2721,31 @@
         <v>43</v>
       </c>
       <c r="B47" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="C47" t="s">
         <v>44</v>
       </c>
       <c r="D47" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E47" t="s">
         <v>103</v>
       </c>
       <c r="F47" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="G47" t="s">
         <v>45</v>
       </c>
       <c r="H47" t="s">
-        <v>84</v>
+        <v>178</v>
       </c>
       <c r="I47" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="J47" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="K47">
         <v>2</v>
@@ -2762,7 +2759,7 @@
         <v>44</v>
       </c>
       <c r="B48" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C48" t="s">
         <v>46</v>
@@ -2774,19 +2771,19 @@
         <v>102</v>
       </c>
       <c r="F48" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="G48" t="s">
         <v>47</v>
       </c>
       <c r="H48" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="I48" t="s">
         <v>108</v>
       </c>
       <c r="J48" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="K48">
         <v>2</v>
@@ -2800,31 +2797,31 @@
         <v>45</v>
       </c>
       <c r="B49" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C49" t="s">
         <v>48</v>
       </c>
       <c r="D49" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="E49" t="s">
         <v>102</v>
       </c>
       <c r="F49" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G49" t="s">
         <v>49</v>
       </c>
       <c r="H49" t="s">
-        <v>181</v>
+        <v>97</v>
       </c>
       <c r="I49" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="J49" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="K49">
         <v>2</v>
@@ -2838,31 +2835,31 @@
         <v>57</v>
       </c>
       <c r="B50" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="C50" t="s">
         <v>50</v>
       </c>
       <c r="D50" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E50" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F50" t="s">
-        <v>22</v>
+        <v>121</v>
       </c>
       <c r="G50" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="H50" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="I50" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="J50" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="K50">
         <v>2</v>
@@ -2876,31 +2873,31 @@
         <v>58</v>
       </c>
       <c r="B51" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="C51" t="s">
         <v>52</v>
       </c>
       <c r="D51" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="E51" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F51" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="G51" t="s">
         <v>53</v>
       </c>
       <c r="H51" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="I51" t="s">
         <v>108</v>
       </c>
       <c r="J51" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="K51">
         <v>2</v>
@@ -2914,31 +2911,31 @@
         <v>59</v>
       </c>
       <c r="B52" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C52" t="s">
         <v>54</v>
       </c>
       <c r="D52" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="E52" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F52" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="G52" t="s">
         <v>55</v>
       </c>
       <c r="H52" t="s">
-        <v>181</v>
+        <v>97</v>
       </c>
       <c r="I52" t="s">
         <v>104</v>
       </c>
       <c r="J52" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="K52">
         <v>2</v>
@@ -2952,31 +2949,31 @@
         <v>60</v>
       </c>
       <c r="B53" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C53" t="s">
         <v>56</v>
       </c>
       <c r="D53" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E53" t="s">
         <v>103</v>
       </c>
       <c r="F53" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G53" t="s">
         <v>57</v>
       </c>
       <c r="H53" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="I53" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="J53" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="K53">
         <v>2</v>
@@ -2990,37 +2987,37 @@
         <v>13</v>
       </c>
       <c r="B54" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="C54" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D54" t="s">
-        <v>97</v>
+        <v>81</v>
       </c>
       <c r="E54" t="s">
-        <v>102</v>
+        <v>111</v>
       </c>
       <c r="F54" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="G54" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H54" t="s">
-        <v>99</v>
+        <v>83</v>
       </c>
       <c r="I54" t="s">
-        <v>111</v>
+        <v>118</v>
       </c>
       <c r="J54" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="K54">
         <v>3</v>
       </c>
       <c r="L54" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="55" spans="1:12">
@@ -3028,31 +3025,31 @@
         <v>14</v>
       </c>
       <c r="B55" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C55" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D55" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E55" t="s">
         <v>104</v>
       </c>
       <c r="F55" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G55" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H55" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="I55" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="J55" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="K55">
         <v>3</v>
@@ -3066,31 +3063,31 @@
         <v>28</v>
       </c>
       <c r="B56" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="C56" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D56" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E56" t="s">
         <v>103</v>
       </c>
       <c r="F56" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="G56" t="s">
         <v>37</v>
       </c>
       <c r="H56" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="I56" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="J56" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="K56">
         <v>3</v>
@@ -3104,31 +3101,31 @@
         <v>29</v>
       </c>
       <c r="B57" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C57" t="s">
         <v>39</v>
       </c>
       <c r="D57" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E57" t="s">
         <v>111</v>
       </c>
       <c r="F57" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G57" t="s">
         <v>41</v>
       </c>
       <c r="H57" t="s">
-        <v>84</v>
+        <v>178</v>
       </c>
       <c r="I57" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="J57" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="K57">
         <v>3</v>
@@ -3142,31 +3139,31 @@
         <v>46</v>
       </c>
       <c r="B58" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="C58" t="s">
         <v>42</v>
       </c>
       <c r="D58" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E58" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F58" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="G58" t="s">
         <v>45</v>
       </c>
       <c r="H58" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I58" t="s">
         <v>111</v>
       </c>
       <c r="J58" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="K58">
         <v>3</v>
@@ -3180,31 +3177,31 @@
         <v>47</v>
       </c>
       <c r="B59" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C59" t="s">
         <v>47</v>
       </c>
       <c r="D59" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E59" t="s">
         <v>108</v>
       </c>
       <c r="F59" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G59" t="s">
         <v>49</v>
       </c>
       <c r="H59" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I59" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="J59" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="K59">
         <v>3</v>
@@ -3218,31 +3215,31 @@
         <v>61</v>
       </c>
       <c r="B60" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="C60" t="s">
         <v>50</v>
       </c>
       <c r="D60" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E60" t="s">
         <v>111</v>
       </c>
       <c r="F60" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="G60" t="s">
         <v>52</v>
       </c>
       <c r="H60" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="I60" t="s">
         <v>102</v>
       </c>
       <c r="J60" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="K60">
         <v>3</v>
@@ -3256,7 +3253,7 @@
         <v>62</v>
       </c>
       <c r="B61" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C61" t="s">
         <v>55</v>
@@ -3268,19 +3265,19 @@
         <v>108</v>
       </c>
       <c r="F61" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G61" t="s">
         <v>57</v>
       </c>
       <c r="H61" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="I61" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="J61" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="K61">
         <v>3</v>
@@ -3294,31 +3291,31 @@
         <v>15</v>
       </c>
       <c r="B62" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="C62" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D62" t="s">
-        <v>58</v>
+        <v>97</v>
       </c>
       <c r="E62" t="s">
+        <v>116</v>
+      </c>
+      <c r="F62" t="s">
+        <v>21</v>
+      </c>
+      <c r="G62" t="s">
+        <v>33</v>
+      </c>
+      <c r="H62" t="s">
+        <v>92</v>
+      </c>
+      <c r="I62" t="s">
         <v>117</v>
       </c>
-      <c r="F62" t="s">
-        <v>22</v>
-      </c>
-      <c r="G62" t="s">
-        <v>34</v>
-      </c>
-      <c r="H62" t="s">
-        <v>160</v>
-      </c>
-      <c r="I62" t="s">
-        <v>104</v>
-      </c>
       <c r="J62" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="K62">
         <v>4</v>
@@ -3332,31 +3329,31 @@
         <v>30</v>
       </c>
       <c r="B63" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="C63" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D63" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E63" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F63" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G63" t="s">
         <v>41</v>
       </c>
       <c r="H63" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="I63" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="J63" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="K63">
         <v>4</v>
@@ -3370,31 +3367,31 @@
         <v>48</v>
       </c>
       <c r="B64" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="C64" t="s">
         <v>42</v>
       </c>
       <c r="D64" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E64" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F64" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G64" t="s">
         <v>49</v>
       </c>
       <c r="H64" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="I64" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="J64" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="K64">
         <v>4</v>
@@ -3408,31 +3405,31 @@
         <v>63</v>
       </c>
       <c r="B65" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="C65" t="s">
         <v>50</v>
       </c>
       <c r="D65" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E65" t="s">
         <v>111</v>
       </c>
       <c r="F65" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G65" t="s">
         <v>57</v>
       </c>
       <c r="H65" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="I65" t="s">
         <v>108</v>
       </c>
       <c r="J65" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="K65">
         <v>4</v>
@@ -3446,31 +3443,31 @@
         <v>31</v>
       </c>
       <c r="B66" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="C66" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D66" t="s">
-        <v>58</v>
+        <v>101</v>
       </c>
       <c r="E66" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F66" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G66" t="s">
         <v>49</v>
       </c>
       <c r="H66" t="s">
-        <v>160</v>
+        <v>85</v>
       </c>
       <c r="I66" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="J66" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="K66">
         <v>5</v>
@@ -3484,31 +3481,31 @@
         <v>33</v>
       </c>
       <c r="B67" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="C67" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D67" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E67" t="s">
         <v>102</v>
       </c>
       <c r="F67" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="G67" t="s">
         <v>50</v>
       </c>
       <c r="H67" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="I67" t="s">
         <v>102</v>
       </c>
       <c r="J67" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="K67">
         <v>5</v>
@@ -3522,37 +3519,37 @@
         <v>32</v>
       </c>
       <c r="B68" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="C68" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D68" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="E68" t="s">
         <v>103</v>
       </c>
       <c r="F68" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="G68" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H68" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="I68" t="s">
-        <v>104</v>
+        <v>119</v>
       </c>
       <c r="J68" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="K68">
         <v>6</v>
       </c>
       <c r="L68" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>